<commit_message>
Refactoring loginPage to SignUp & loginTests to signUpTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atif Zulfiqar Malik\IdeaProjects\AppiumSession3\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Appium_Java_Training\booking.com_App\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16581F2E-2021-4FCC-B719-D80C9C5AE215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122789EB-ACAB-49E4-80F2-483AEC31F43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F008BE4-AB88-4FFD-A1DF-09969BB15F96}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>test@yopmail.com</t>
+    <t>Test$1234!</t>
   </si>
   <si>
-    <t>Test$1234!</t>
+    <t>yes@finalmail.com</t>
   </si>
 </sst>
 </file>
@@ -421,10 +421,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding searchPage and searchTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Appium_Java_Training\booking.com_App\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122789EB-ACAB-49E4-80F2-483AEC31F43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4707C3C3-6B89-41E2-B057-F8DB3814B4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F008BE4-AB88-4FFD-A1DF-09969BB15F96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Test$1234!</t>
   </si>
   <si>
-    <t>yes@finalmail.com</t>
+    <t>best@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>